<commit_message>
feat: Mejorar la visibilidad del sidebar en dispositivos móviles
</commit_message>
<xml_diff>
--- a/uploads/1/quinta.xlsx
+++ b/uploads/1/quinta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\app_auditorias\uploads\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642E93E5-5DC0-4CD4-A272-4ACFB4679E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D3D96A-1817-47DD-A3C7-6BFE07568B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A17DF12A-74E1-4423-B87C-A4AF74AA687A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Proyecto E SAS</t>
   </si>
@@ -86,9 +86,6 @@
     <t>CanAmor - Shampoo Arbol De Te Gatos - 230 MILILITRO</t>
   </si>
   <si>
-    <t>PD400000126</t>
-  </si>
-  <si>
     <t>Paw Day - Juguete Mordedor Interactivo Pato - ROJO</t>
   </si>
   <si>
@@ -147,9 +144,6 @@
   </si>
   <si>
     <t>052742930107</t>
-  </si>
-  <si>
-    <t>6920300000262</t>
   </si>
   <si>
     <t>7708228519115</t>
@@ -724,7 +718,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="42" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -752,6 +746,9 @@
     </xf>
     <xf numFmtId="4" fontId="22" fillId="0" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1137,65 +1134,68 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AF0D48D-248A-4D6C-B62F-F17038EAD2ED}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.4">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.4">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.4">
-      <c r="A5" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
+      <c r="A5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.4">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
@@ -1226,7 +1226,7 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="6"/>
       <c r="B9" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>11</v>
@@ -1241,7 +1241,7 @@
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="6"/>
       <c r="B10" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>12</v>
@@ -1255,8 +1255,8 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="6"/>
-      <c r="B11" s="3" t="s">
-        <v>37</v>
+      <c r="B11" s="10">
+        <v>6291104080010</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>13</v>
@@ -1271,7 +1271,7 @@
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
       <c r="B12" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>14</v>
@@ -1286,7 +1286,7 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="6"/>
       <c r="B13" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>15</v>
@@ -1300,11 +1300,11 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="6"/>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="10">
+        <v>7702045320619</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="D14" s="4">
         <v>4</v>
@@ -1316,10 +1316,10 @@
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="6"/>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" s="4">
         <v>2</v>
@@ -1331,10 +1331,10 @@
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="6"/>
       <c r="B16" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
@@ -1346,10 +1346,10 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="6"/>
       <c r="B17" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="4">
         <v>2</v>
@@ -1361,10 +1361,10 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="6"/>
       <c r="B18" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18" s="4">
         <v>20</v>
@@ -1376,10 +1376,10 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="6"/>
       <c r="B19" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" s="4">
         <v>8</v>
@@ -1391,10 +1391,10 @@
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="6"/>
       <c r="B20" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" s="4">
         <v>6</v>
@@ -1406,10 +1406,10 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="6"/>
       <c r="B21" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D21" s="4">
         <v>8</v>
@@ -1421,10 +1421,10 @@
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="6"/>
       <c r="B22" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" s="4">
         <v>5</v>
@@ -1436,10 +1436,10 @@
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="6"/>
       <c r="B23" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D23" s="4">
         <v>24</v>
@@ -1451,10 +1451,10 @@
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="6"/>
       <c r="B24" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24" s="4">
         <v>7</v>
@@ -1466,10 +1466,10 @@
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="6"/>
       <c r="B25" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D25" s="4">
         <v>1</v>
@@ -1481,10 +1481,10 @@
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="6"/>
       <c r="B26" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D26" s="4">
         <v>18</v>
@@ -1496,10 +1496,10 @@
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
       <c r="B27" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D27" s="4">
         <v>22</v>
@@ -1510,7 +1510,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -1523,7 +1523,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -1536,7 +1536,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>

</xml_diff>